<commit_message>
* Swapped order of series in matrix chart * wrote CPU implementation chapter of matrix mul
</commit_message>
<xml_diff>
--- a/results/2013_01_08_mult.xlsx
+++ b/results/2013_01_08_mult.xlsx
@@ -1758,15 +1758,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="8"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>stats!$A$168:$B$168</c:f>
+              <c:f>stats!$A$222:$B$222</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Matrix multiplication (Tiles, AMD) GPU CL</c:v>
+                  <c:v>Matrix multiplication (NVIDIA) GPU CL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1776,7 +1776,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>stats!$A$170:$A$193</c:f>
+              <c:f>stats!$A$224:$A$247</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -1857,81 +1857,81 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>stats!$K$170:$K$193</c:f>
+              <c:f>stats!$K$224:$K$247</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>3.2919999999999998E-3</c:v>
+                  <c:v>3.31E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9970000000000001E-3</c:v>
+                  <c:v>3.0860000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2109999999999999E-3</c:v>
+                  <c:v>3.2200000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9280000000000001E-3</c:v>
+                  <c:v>3.5370000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.7260000000000001E-3</c:v>
+                  <c:v>3.5920000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7079999999999999E-3</c:v>
+                  <c:v>4.5339999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1409999999999997E-3</c:v>
+                  <c:v>8.1010000000000006E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.444E-3</c:v>
+                  <c:v>1.0392E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.443E-3</c:v>
+                  <c:v>1.7936000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.757E-3</c:v>
+                  <c:v>2.7938000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.374E-2</c:v>
+                  <c:v>4.0325E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6292000000000001E-2</c:v>
+                  <c:v>5.5882000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4514000000000001E-2</c:v>
+                  <c:v>8.0987000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9454999999999999E-2</c:v>
+                  <c:v>0.111748</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8647000000000001E-2</c:v>
+                  <c:v>0.19247</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1888000000000002E-2</c:v>
+                  <c:v>0.21786700000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1075999999999998E-2</c:v>
+                  <c:v>0.35493200000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.8904000000000007E-2</c:v>
+                  <c:v>0.32865800000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.8782E-2</c:v>
+                  <c:v>0.40837200000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9732999999999993E-2</c:v>
+                  <c:v>0.58086099999999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.12314700000000001</c:v>
+                  <c:v>0.56536600000000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.14690400000000001</c:v>
+                  <c:v>0.65603500000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.16642999999999999</c:v>
+                  <c:v>0.79637800000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.21995899999999999</c:v>
+                  <c:v>0.93823699999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2120,15 +2120,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
+          <c:idx val="6"/>
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>stats!$A$222:$B$222</c:f>
+              <c:f>stats!$A$168:$B$168</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Matrix multiplication (NVIDIA) GPU CL</c:v>
+                  <c:v>Matrix multiplication (Tiles, AMD) GPU CL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2138,7 +2138,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>stats!$A$224:$A$247</c:f>
+              <c:f>stats!$A$170:$A$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
@@ -2219,81 +2219,81 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>stats!$K$224:$K$247</c:f>
+              <c:f>stats!$K$170:$K$193</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>3.31E-3</c:v>
+                  <c:v>3.2919999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0860000000000002E-3</c:v>
+                  <c:v>2.9970000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2200000000000002E-3</c:v>
+                  <c:v>3.2109999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.5370000000000002E-3</c:v>
+                  <c:v>4.9280000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.5920000000000001E-3</c:v>
+                  <c:v>2.7260000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5339999999999998E-3</c:v>
+                  <c:v>3.7079999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.1010000000000006E-3</c:v>
+                  <c:v>4.1409999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0392E-2</c:v>
+                  <c:v>4.444E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7936000000000001E-2</c:v>
+                  <c:v>7.443E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7938000000000001E-2</c:v>
+                  <c:v>9.757E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0325E-2</c:v>
+                  <c:v>1.374E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.5882000000000001E-2</c:v>
+                  <c:v>1.6292000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.0987000000000003E-2</c:v>
+                  <c:v>2.4514000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.111748</c:v>
+                  <c:v>2.9454999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.19247</c:v>
+                  <c:v>3.8647000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.21786700000000001</c:v>
+                  <c:v>4.1888000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.35493200000000003</c:v>
+                  <c:v>6.1075999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.32865800000000001</c:v>
+                  <c:v>6.8904000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.40837200000000001</c:v>
+                  <c:v>8.8782E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.58086099999999996</c:v>
+                  <c:v>8.9732999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.56536600000000004</c:v>
+                  <c:v>0.12314700000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.65603500000000003</c:v>
+                  <c:v>0.14690400000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.79637800000000003</c:v>
+                  <c:v>0.16642999999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.93823699999999999</c:v>
+                  <c:v>0.21995899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2308,11 +2308,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="106748096"/>
-        <c:axId val="106748672"/>
+        <c:axId val="40245440"/>
+        <c:axId val="40246016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106748096"/>
+        <c:axId val="40245440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -2323,12 +2323,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106748672"/>
+        <c:crossAx val="40246016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106748672"/>
+        <c:axId val="40246016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2340,7 +2340,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106748096"/>
+        <c:crossAx val="40245440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2664,11 +2664,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73528832"/>
-        <c:axId val="141001856"/>
+        <c:axId val="43032576"/>
+        <c:axId val="40241408"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="73528832"/>
+        <c:axId val="43032576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2677,7 +2677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="141001856"/>
+        <c:crossAx val="40241408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2685,7 +2685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141001856"/>
+        <c:axId val="40241408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2696,14 +2696,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73528832"/>
+        <c:crossAx val="43032576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3044,11 +3043,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43950592"/>
-        <c:axId val="44144256"/>
+        <c:axId val="43033088"/>
+        <c:axId val="40244864"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="43950592"/>
+        <c:axId val="43033088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3057,7 +3056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44144256"/>
+        <c:crossAx val="40244864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3065,7 +3064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44144256"/>
+        <c:axId val="40244864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3076,14 +3075,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43950592"/>
+        <c:crossAx val="43033088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3482,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U41" sqref="U41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>